<commit_message>
se termino de agregar la collection
</commit_message>
<xml_diff>
--- a/configs/db/negocios.xlsx
+++ b/configs/db/negocios.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Empresas" state="visible" r:id="rId4"/>
+    <sheet name="Empresas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nombre</t>
   </si>
@@ -25,23 +28,34 @@
     <t>Categoria</t>
   </si>
   <si>
-    <t>Empresa nivel pueblito</t>
-  </si>
-  <si>
-    <t>22</t>
+    <t>Empresa cooperativa</t>
+  </si>
+  <si>
+    <t>cooperativa</t>
+  </si>
+  <si>
+    <t>UniveresalRods</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,8 +78,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -84,7 +100,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -94,44 +110,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -161,12 +177,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -205,208 +221,160 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -422,19 +390,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>